<commit_message>
Final Updated Data Done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -182,132 +182,87 @@
     <t>Faults Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Added Data\OM13_Faults_Data.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for Original Faults Data to Work With</t>
   </si>
   <si>
     <t>Intermediate_Faults_Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Intermediate Data\Faults_Data.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for Faults Data to Work With, to follow good practice so that original file remains the same.</t>
   </si>
   <si>
     <t>Actual Part Code Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Added Data\FFR Data Actual Part with Part code.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for Excel which contains all consolidated parts in it for vlookup</t>
   </si>
   <si>
     <t>Error Handling Faults Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Exception Handling Folder\Faults_Data.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for Error Handling</t>
   </si>
   <si>
     <t>Population Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Added Data\AC - IW POP OM1_21 TO OM13_21.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for Population Data to Work With</t>
   </si>
   <si>
     <t>Intermediate Population Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Intermediate Data\Population Data.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for Population Data to Work With, to follow good practice so that original file remains the same.</t>
   </si>
   <si>
     <t>Error Handling Population Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Exception Handling Folder\Population Data.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for Error Handling, This Must be a Empty File</t>
   </si>
   <si>
     <t>Master Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Added Data\Master  In Warranty Population Vs  Complaints OM12 2022.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for AC FFR Models Data to Work With</t>
   </si>
   <si>
     <t>Intermediate Master Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Intermediate Data\AC FFR Models.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for AC FFR Models Data to Work With, to follow good practice so that original file remains the same.</t>
   </si>
   <si>
     <t>Error Handling AC Models Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Exception Handling Folder\AC FFR Models.xlsx</t>
-  </si>
-  <si>
     <t>FFR_Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Added Data\FFR_Data.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for AC FFR Data to Work With</t>
   </si>
   <si>
     <t>Intermediate FFR_Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Intermediate Data\FFR_Data.xlsx</t>
-  </si>
-  <si>
     <t>Provide File Path for AC FFR Data to Work With, to follow good practice so that original file remains the same.</t>
   </si>
   <si>
     <t>Presentation Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Intermediate Data\AC FFR PPT.pptx</t>
-  </si>
-  <si>
     <t>Provide the path where you want your file to run</t>
   </si>
   <si>
     <t>Error Handling Presentation Data</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Exception Handling Folder\AC FFR OM08.pptx</t>
-  </si>
-  <si>
     <t>Provide the Empty file Path if Any Error occurs</t>
   </si>
   <si>
     <t>Final Data Path</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\Final Data</t>
-  </si>
-  <si>
     <t>Where You Want All Your Finalised Data</t>
   </si>
   <si>
@@ -320,81 +275,42 @@
     <t>AddingLineGraph</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\AddingLineGraph.vbs</t>
-  </si>
-  <si>
     <t>AutofitColumn</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\AutofitColumn.vbs</t>
-  </si>
-  <si>
     <t>DeleteSheets</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\DeleteSheets.vbs</t>
-  </si>
-  <si>
     <t>Graph</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\Graph.vbs</t>
-  </si>
-  <si>
     <t>Merge</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\Merge.vbs</t>
-  </si>
-  <si>
     <t>NewSheet</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\NewSheet.vbs</t>
-  </si>
-  <si>
     <t>NewTableGraphBorder</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\NewTableGraphBorder.vbs</t>
-  </si>
-  <si>
     <t>OneTableGraphBorder</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\OneTableGraphBorder.vbs</t>
-  </si>
-  <si>
     <t>ThreeTableGraphBorder</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\ThreeTableGraphBorder.vbs</t>
-  </si>
-  <si>
     <t>TwoTableGraphBorder</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\TwoTableGraphBorder.vbs</t>
-  </si>
-  <si>
     <t>Unmerge</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\Unmerge.vbs</t>
-  </si>
-  <si>
     <t>UpdateChart</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\UpdateChart.vbs</t>
-  </si>
-  <si>
     <t>ZoomOut</t>
   </si>
   <si>
-    <t>C:\Users\gaura\Desktop\FFR Data\FFR VB Script\ZoomOut.vbs</t>
-  </si>
-  <si>
     <t>OM Month Data</t>
   </si>
   <si>
@@ -420,6 +336,90 @@
   </si>
   <si>
     <t>Data\Output\Output Results.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\OM13_Faults_Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Intermediate Data\Faults_Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\FFR Data Actual Part with Part code.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Exception Handling Folder\Faults_Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\AC - IW POP OM1_21 TO OM13_21.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Intermediate Data\Population Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Exception Handling Folder\Population Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\Master  In Warranty Population Vs  Complaints OM12 2022.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Intermediate Data\AC FFR Models.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Exception Handling Folder\AC FFR Models.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\FFR_Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Intermediate Data\FFR_Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Intermediate Data\AC FFR PPT.pptx</t>
+  </si>
+  <si>
+    <t>FFR Data\Exception Handling Folder\AC FFR OM08.pptx</t>
+  </si>
+  <si>
+    <t>FFR Data\Final Data</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\AddingLineGraph.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\AutofitColumn.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\DeleteSheets.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\Graph.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\Merge.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\NewSheet.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\NewTableGraphBorder.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\OneTableGraphBorder.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\ThreeTableGraphBorder.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\TwoTableGraphBorder.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\Unmerge.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\UpdateChart.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\ZoomOut.vbs</t>
   </si>
 </sst>
 </file>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -896,10 +896,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -936,10 +936,10 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C13" s="5"/>
     </row>
@@ -948,43 +948,43 @@
         <v>51</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -999,44 +999,44 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -1051,44 +1051,44 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -1103,31 +1103,31 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
@@ -1137,31 +1137,31 @@
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
@@ -1171,13 +1171,13 @@
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
@@ -1187,10 +1187,10 @@
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C42" s="5"/>
     </row>
@@ -1201,118 +1201,118 @@
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="5" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" s="5" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" s="5" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>122</v>
+        <v>94</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="C56" s="5"/>
     </row>
@@ -1320,10 +1320,10 @@
     <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" s="10" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
All Finalised and Done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +53,6 @@
     <t>LogMessage_GetTransactionData</t>
   </si>
   <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
     <t>LogMessage_GetTransactionDataError</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -164,9 +158,6 @@
     <t>Previous_OM_Month</t>
   </si>
   <si>
-    <t>OM12</t>
-  </si>
-  <si>
     <t>Add Previous Month FFR value as OM01,OM02,OM03,…..,OM13</t>
   </si>
   <si>
@@ -338,9 +329,6 @@
     <t>Data\Output\Output Results.xlsx</t>
   </si>
   <si>
-    <t>FFR Data\Added Data\OM13_Faults_Data.xlsx</t>
-  </si>
-  <si>
     <t>FFR Data\Intermediate Data\Faults_Data.xlsx</t>
   </si>
   <si>
@@ -350,18 +338,12 @@
     <t>FFR Data\Exception Handling Folder\Faults_Data.xlsx</t>
   </si>
   <si>
-    <t>FFR Data\Added Data\AC - IW POP OM1_21 TO OM13_21.xlsx</t>
-  </si>
-  <si>
     <t>FFR Data\Intermediate Data\Population Data.xlsx</t>
   </si>
   <si>
     <t>FFR Data\Exception Handling Folder\Population Data.xlsx</t>
   </si>
   <si>
-    <t>FFR Data\Added Data\Master  In Warranty Population Vs  Complaints OM12 2022.xlsx</t>
-  </si>
-  <si>
     <t>FFR Data\Intermediate Data\AC FFR Models.xlsx</t>
   </si>
   <si>
@@ -420,6 +402,33 @@
   </si>
   <si>
     <t>FFR Data\FFR VB Script\ZoomOut.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\OM01 Faults Data.xlsx</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\IW POP AC OM1_22-23 to OM2_22-23.xlsx</t>
+  </si>
+  <si>
+    <t>OM01</t>
+  </si>
+  <si>
+    <t>FFR Data\Added Data\OM13_Masters_Data.xlsx</t>
+  </si>
+  <si>
+    <t>GFD Send Data</t>
+  </si>
+  <si>
+    <t>For_Population</t>
+  </si>
+  <si>
+    <t>OM1</t>
+  </si>
+  <si>
+    <t>For Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction For Model - </t>
   </si>
 </sst>
 </file>
@@ -808,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -858,34 +867,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -896,38 +905,44 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="5"/>
@@ -935,62 +950,62 @@
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>105</v>
+        <v>48</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="5"/>
@@ -998,51 +1013,51 @@
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="A21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>109</v>
+        <v>56</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="5"/>
@@ -1050,51 +1065,51 @@
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="A27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>112</v>
+        <v>62</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="A30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" s="5"/>
@@ -1102,228 +1117,236 @@
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>100</v>
-      </c>
+      <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="A33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="A35" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" s="6" t="s">
-        <v>101</v>
-      </c>
+      <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="A37" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" s="5" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="7"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>131</v>
+        <v>90</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="C56" s="5"/>
     </row>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="5"/>
+    </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2270,7 +2293,6 @@
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
-    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2282,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2336,18 +2358,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2368,100 +2390,100 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3465,7 +3487,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added Invoke VBA for Copying Chart and Table
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -429,6 +429,18 @@
   </si>
   <si>
     <t xml:space="preserve">Processing Transaction For Model - </t>
+  </si>
+  <si>
+    <t>CopyingTable</t>
+  </si>
+  <si>
+    <t>CopyingChart</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\Copying_Chart.vbs</t>
+  </si>
+  <si>
+    <t>FFR Data\FFR VB Script\Copying_Table.vbs</t>
   </si>
 </sst>
 </file>
@@ -817,16 +829,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -1340,17 +1352,33 @@
       </c>
       <c r="C57" s="5"/>
     </row>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A58" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="5"/>
+    </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A61" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B61" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2293,6 +2321,8 @@
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2304,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>